<commit_message>
update to CakePHP 3.6
</commit_message>
<xml_diff>
--- a/webroot/files/contact_csv-import.xlsx
+++ b/webroot/files/contact_csv-import.xlsx
@@ -1,17 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="206"/>
-  </bookViews>
-  <sheets>
-    <sheet name="contacts-csv-import" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-</workbook>
-</file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -153,266 +139,6 @@
 </comments>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
-  <si>
-    <t>contactname</t>
-  </si>
-  <si>
-    <t>legalname</t>
-  </si>
-  <si>
-    <t>zip</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>birth</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>workplace</t>
-  </si>
-  <si>
-    <t>workplace_zip</t>
-  </si>
-  <si>
-    <t>workplace_address</t>
-  </si>
-  <si>
-    <t>workplace_phone</t>
-  </si>
-  <si>
-    <t>workplace_email</t>
-  </si>
-  <si>
-    <t>contactsource_id</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>skills</t>
-  </si>
-  <si>
-    <t>groups</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>születési név</t>
-  </si>
-  <si>
-    <t>taj</t>
-  </si>
-  <si>
-    <t>Acyuta Isvara</t>
-  </si>
-  <si>
-    <t>Kovács Attila</t>
-  </si>
-  <si>
-    <t>Radha-Krisna krt. 2.</t>
-  </si>
-  <si>
-    <t>1991-04-06 00:00:00</t>
-  </si>
-  <si>
-    <t>7,5,6</t>
-  </si>
-  <si>
-    <t>043-903-087</t>
-  </si>
-  <si>
-    <t>Liget Nóra</t>
-  </si>
-  <si>
-    <t>7838 Piskó</t>
-  </si>
-  <si>
-    <t>Fő u 10</t>
-  </si>
-  <si>
-    <t>1989-01-23 00:00:00</t>
-  </si>
-  <si>
-    <t>091-127-589</t>
-  </si>
-  <si>
-    <t>Pesti Andi</t>
-  </si>
-  <si>
-    <t>Pesti Andrea</t>
-  </si>
-  <si>
-    <t>7838 Vejti</t>
-  </si>
-  <si>
-    <t>Fő u 2</t>
-  </si>
-  <si>
-    <t>1994-09-26 00:00:00</t>
-  </si>
-  <si>
-    <t>108-626-296</t>
-  </si>
-  <si>
-    <t>5,-3</t>
-  </si>
-</sst>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-  </fonts>
-  <fills count="3">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF99"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFF99"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -846,291 +572,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>